<commit_message>
Added App Notes of GSM Module. Added requirements
</commit_message>
<xml_diff>
--- a/Docs/Requirements.xlsx
+++ b/Docs/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\russel\Documents\Embedded\projects\garbage_monitor\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C793A7BA-F8E4-4BF7-8B4E-642BE062E3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38503A52-AE81-49BA-9F81-D40927A2F6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15750" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Req" sheetId="1" r:id="rId1"/>
@@ -583,7 +583,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added docs for components
</commit_message>
<xml_diff>
--- a/Docs/Requirements.xlsx
+++ b/Docs/Requirements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\russel\Documents\Embedded\projects\garbage_monitor\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38503A52-AE81-49BA-9F81-D40927A2F6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A269B3-F6C7-43C7-8465-8311F6D62D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Customer Req" sheetId="1" r:id="rId1"/>
     <sheet name="Technical Specs" sheetId="2" r:id="rId2"/>
     <sheet name="Functional Req" sheetId="3" r:id="rId3"/>
-    <sheet name="Non-Functional Req" sheetId="4" r:id="rId4"/>
+    <sheet name="Data" sheetId="5" r:id="rId4"/>
+    <sheet name="Non-Functional Req" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>The level of trash inside the bin can be monitored using internet</t>
   </si>
@@ -57,9 +58,6 @@
     <t>The installer can trigger the device to transmit data to internet</t>
   </si>
   <si>
-    <t>When 12 hours is elapsed since the last transmission of the sensor data (trash level, orientation, temperature, humidity, location), the device will transmit the current sensor data.</t>
-  </si>
-  <si>
     <t>When the transmit button is pressed, the device will transmit the current sensor data.</t>
   </si>
   <si>
@@ -75,12 +73,6 @@
     <t>When the trash level reached a certain level, the device will send alert to SMS and Email</t>
   </si>
   <si>
-    <t>When fire is detected, user should be notified via email and SMS</t>
-  </si>
-  <si>
-    <t>When the potential fire is detected, the device will send alert to SMS and Email</t>
-  </si>
-  <si>
     <t>When the device is not calibrated, it will blink an LED at 1 Hz rate</t>
   </si>
   <si>
@@ -88,6 +80,72 @@
   </si>
   <si>
     <t>When the calibration button is pressed, the device will be calibrated and the LED will be -turned off</t>
+  </si>
+  <si>
+    <t>Fill Level</t>
+  </si>
+  <si>
+    <t>0 - 100</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>unsigned int</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Orientation</t>
+  </si>
+  <si>
+    <t>0 - 360</t>
+  </si>
+  <si>
+    <t>Degrees</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Location_GPS</t>
+  </si>
+  <si>
+    <t>Location_GSM</t>
+  </si>
+  <si>
+    <t>The device will use the Cellular Base station on determining position in case the GPS cannot get a fix</t>
+  </si>
+  <si>
+    <t>When 12 hours is elapsed since the last transmission of the sensor data (trash level, orientation,location), the device will transmit the current sensor data.</t>
+  </si>
+  <si>
+    <t>Calibration Status</t>
+  </si>
+  <si>
+    <t>Signal Level</t>
+  </si>
+  <si>
+    <t>true,false</t>
+  </si>
+  <si>
+    <t>dbm</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>bool</t>
   </si>
 </sst>
 </file>
@@ -449,7 +507,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -473,16 +531,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{766D5319-F687-4E01-8D30-7AED793F20DC}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="83.85546875" customWidth="1"/>
+    <col min="2" max="2" width="93.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -498,7 +556,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -506,12 +564,12 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -519,57 +577,49 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -580,10 +630,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E86DFF-D7E6-4247-B4C2-9D28D610FACE}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,12 +642,12 @@
     <col min="2" max="2" width="92.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -605,7 +655,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -613,7 +663,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -621,7 +671,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -629,7 +679,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -637,15 +687,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -654,10 +696,113 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1199B11-0EA8-44A1-8355-5D8A0D32CDD4}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFAF775-551F-4016-BC33-B5957DAA50D7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>